<commit_message>
Curate the data folder
</commit_message>
<xml_diff>
--- a/data/regs/indiana.xlsx
+++ b/data/regs/indiana.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bcp322\Box\Personal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/palsb1/Library/CloudStorage/Box-Box/researchB/online_version_JAERE/data/Bridget/use_data/regulations/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B25EB49-5B4B-D048-AD38-8114EADB2613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12225" yWindow="2355" windowWidth="14685" windowHeight="14475"/>
+    <workbookView xWindow="2360" yWindow="900" windowWidth="24620" windowHeight="14480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Data Dictionary" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="108">
   <si>
     <t>Plant Name</t>
   </si>
@@ -317,13 +319,55 @@
   </si>
   <si>
     <t>65 Fed. Reg. 52315, 52316 (Aug. 29, 2000); 54 Fed. Reg. 2112 (Jan. 19, 1989) (final rule); 53 Fed. Reg. 34310, 34313 (Sept. 6, 1988) (proposed rule)</t>
+  </si>
+  <si>
+    <t>PLEASE NOTE: This file was generated based on the coal boilers that appeared in our dataset.  It is therefore NOT necessarily a full accounting of all coal boiler regulations in Indiana.</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>This variable provides the page number in article7_11-2021.pdf (provided in zip folder) where the regulation is provided.</t>
+  </si>
+  <si>
+    <t>This variable indicates the end period of the regulation's effectiveness.</t>
+  </si>
+  <si>
+    <t>This variable indicates the start period of the regulation's effectiveness.</t>
+  </si>
+  <si>
+    <t>This variable provides the county of the plant.</t>
+  </si>
+  <si>
+    <t>This variable provides additional sources (outside of article7_11-2021.pdf) that were used to determine the parameters of the regulation.</t>
+  </si>
+  <si>
+    <t>This variable indicates any additional limits on the boiler.</t>
+  </si>
+  <si>
+    <t>This variable indicates the emission limit of the boiler.</t>
+  </si>
+  <si>
+    <t>This variable provides, where applicable, the generator ID subject to the regulation.</t>
+  </si>
+  <si>
+    <t>This variable provides, where applicable, the ID of the boiler subject to the regulation.</t>
+  </si>
+  <si>
+    <t>This variable provides the plant code of the plant subject to the regulation.</t>
+  </si>
+  <si>
+    <t>This variable provides the name of the plant subject to the regulation.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -350,8 +394,24 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -364,8 +424,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -373,11 +445,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -392,8 +479,25 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -707,26 +811,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.875" customWidth="1"/>
-    <col min="5" max="5" width="10.875" style="9"/>
-    <col min="8" max="8" width="10.875" style="4"/>
-    <col min="9" max="9" width="13.875" customWidth="1"/>
+    <col min="1" max="1" width="22.83203125" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="9"/>
+    <col min="8" max="8" width="10.83203125" style="4"/>
+    <col min="9" max="9" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -761,7 +865,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -787,7 +891,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -813,7 +917,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -839,7 +943,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -862,7 +966,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -885,7 +989,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -908,7 +1012,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -931,7 +1035,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -957,7 +1061,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -983,7 +1087,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1006,7 +1110,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1032,7 +1136,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -1061,7 +1165,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1090,7 +1194,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -1116,7 +1220,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -1142,7 +1246,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>12</v>
       </c>
@@ -1172,7 +1276,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>12</v>
       </c>
@@ -1202,7 +1306,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>12</v>
       </c>
@@ -1232,7 +1336,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>12</v>
       </c>
@@ -1262,7 +1366,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>12</v>
       </c>
@@ -1292,7 +1396,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>12</v>
       </c>
@@ -1322,7 +1426,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>12</v>
       </c>
@@ -1350,7 +1454,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>13</v>
       </c>
@@ -1373,15 +1477,15 @@
       <c r="H26" s="4">
         <v>1999</v>
       </c>
-      <c r="I26" s="13"/>
-      <c r="J26" s="12" t="s">
+      <c r="I26" s="1"/>
+      <c r="J26" t="s">
         <v>28</v>
       </c>
-      <c r="K26" s="12" t="s">
+      <c r="K26" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>13</v>
       </c>
@@ -1404,15 +1508,15 @@
       <c r="H27" s="4">
         <v>1999</v>
       </c>
-      <c r="I27" s="13"/>
-      <c r="J27" s="12" t="s">
+      <c r="I27" s="1"/>
+      <c r="J27" t="s">
         <v>28</v>
       </c>
-      <c r="K27" s="12" t="s">
+      <c r="K27" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>13</v>
       </c>
@@ -1432,15 +1536,15 @@
       <c r="H28" s="4">
         <v>1999</v>
       </c>
-      <c r="I28" s="13"/>
-      <c r="J28" s="12" t="s">
+      <c r="I28" s="1"/>
+      <c r="J28" t="s">
         <v>28</v>
       </c>
-      <c r="K28" s="12" t="s">
+      <c r="K28" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>13</v>
       </c>
@@ -1460,15 +1564,15 @@
       <c r="H29" s="4">
         <v>1999</v>
       </c>
-      <c r="I29" s="13"/>
-      <c r="J29" s="12" t="s">
+      <c r="I29" s="1"/>
+      <c r="J29" t="s">
         <v>28</v>
       </c>
-      <c r="K29" s="12" t="s">
+      <c r="K29" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>13</v>
       </c>
@@ -1498,7 +1602,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>13</v>
       </c>
@@ -1528,7 +1632,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>13</v>
       </c>
@@ -1558,7 +1662,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>13</v>
       </c>
@@ -1588,7 +1692,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>15</v>
       </c>
@@ -1616,7 +1720,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>15</v>
       </c>
@@ -1647,7 +1751,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>15</v>
       </c>
@@ -1677,7 +1781,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>15</v>
       </c>
@@ -1701,7 +1805,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>15</v>
       </c>
@@ -1728,7 +1832,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>15</v>
       </c>
@@ -1755,7 +1859,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>16</v>
       </c>
@@ -1772,15 +1876,14 @@
       <c r="G40" s="1">
         <v>2017</v>
       </c>
-      <c r="I40" s="12">
+      <c r="I40">
         <v>15</v>
       </c>
-      <c r="J40" s="12" t="s">
+      <c r="J40" t="s">
         <v>5</v>
       </c>
-      <c r="K40" s="12"/>
-    </row>
-    <row r="41" spans="1:11">
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>16</v>
       </c>
@@ -1797,15 +1900,14 @@
       <c r="G41" s="1">
         <v>2017</v>
       </c>
-      <c r="I41" s="12">
+      <c r="I41">
         <v>15</v>
       </c>
-      <c r="J41" s="12" t="s">
+      <c r="J41" t="s">
         <v>5</v>
       </c>
-      <c r="K41" s="12"/>
-    </row>
-    <row r="42" spans="1:11">
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>16</v>
       </c>
@@ -1822,15 +1924,14 @@
       <c r="G42" s="1">
         <v>2017</v>
       </c>
-      <c r="I42" s="12">
+      <c r="I42">
         <v>15</v>
       </c>
-      <c r="J42" s="12" t="s">
+      <c r="J42" t="s">
         <v>5</v>
       </c>
-      <c r="K42" s="12"/>
-    </row>
-    <row r="43" spans="1:11">
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>17</v>
       </c>
@@ -1860,7 +1961,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>17</v>
       </c>
@@ -1890,7 +1991,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>17</v>
       </c>
@@ -1920,7 +2021,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>17</v>
       </c>
@@ -1950,7 +2051,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>17</v>
       </c>
@@ -1980,7 +2081,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>17</v>
       </c>
@@ -2013,7 +2114,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="49" spans="1:11">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>17</v>
       </c>
@@ -2046,7 +2147,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="50" spans="1:11">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>17</v>
       </c>
@@ -2079,7 +2180,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>17</v>
       </c>
@@ -2112,7 +2213,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>17</v>
       </c>
@@ -2142,7 +2243,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>17</v>
       </c>
@@ -2172,7 +2273,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="54" spans="1:11">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>17</v>
       </c>
@@ -2202,7 +2303,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="55" spans="1:11">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>17</v>
       </c>
@@ -2232,7 +2333,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="56" spans="1:11">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>17</v>
       </c>
@@ -2262,7 +2363,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="57" spans="1:11">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>17</v>
       </c>
@@ -2289,7 +2390,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="58" spans="1:11">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>17</v>
       </c>
@@ -2316,7 +2417,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="1:11">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>17</v>
       </c>
@@ -2343,7 +2444,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="60" spans="1:11">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>17</v>
       </c>
@@ -2370,7 +2471,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:11">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>17</v>
       </c>
@@ -2397,7 +2498,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:11">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>67</v>
       </c>
@@ -2424,7 +2525,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="1:11">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>67</v>
       </c>
@@ -2451,7 +2552,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="64" spans="1:11">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>67</v>
       </c>
@@ -2478,7 +2579,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="65" spans="1:11">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>67</v>
       </c>
@@ -2505,7 +2606,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="66" spans="1:11">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>67</v>
       </c>
@@ -2532,7 +2633,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="67" spans="1:11">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>67</v>
       </c>
@@ -2559,7 +2660,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="68" spans="1:11">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>67</v>
       </c>
@@ -2586,7 +2687,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="69" spans="1:11">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>67</v>
       </c>
@@ -2613,7 +2714,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:11">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>67</v>
       </c>
@@ -2640,7 +2741,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:11">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>67</v>
       </c>
@@ -2667,7 +2768,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="72" spans="1:11">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>14</v>
       </c>
@@ -2691,7 +2792,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="73" spans="1:11">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>14</v>
       </c>
@@ -2715,7 +2816,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="74" spans="1:11">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>63</v>
       </c>
@@ -2742,7 +2843,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="75" spans="1:11">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>63</v>
       </c>
@@ -2762,15 +2863,14 @@
       <c r="H75" s="4">
         <v>2001</v>
       </c>
-      <c r="I75" s="12"/>
-      <c r="J75" s="13" t="s">
+      <c r="J75" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K75" s="12" t="s">
+      <c r="K75" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="76" spans="1:11">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>63</v>
       </c>
@@ -2790,15 +2890,14 @@
       <c r="H76" s="4">
         <v>2001</v>
       </c>
-      <c r="I76" s="12"/>
-      <c r="J76" s="13" t="s">
+      <c r="J76" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K76" s="12" t="s">
+      <c r="K76" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="77" spans="1:11">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>63</v>
       </c>
@@ -2818,15 +2917,14 @@
       <c r="H77" s="4">
         <v>2001</v>
       </c>
-      <c r="I77" s="12"/>
-      <c r="J77" s="13" t="s">
+      <c r="J77" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K77" s="12" t="s">
+      <c r="K77" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="78" spans="1:11">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>63</v>
       </c>
@@ -2846,15 +2944,14 @@
       <c r="H78" s="4">
         <v>2001</v>
       </c>
-      <c r="I78" s="12"/>
-      <c r="J78" s="13" t="s">
+      <c r="J78" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K78" s="12" t="s">
+      <c r="K78" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="79" spans="1:11">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>63</v>
       </c>
@@ -2874,15 +2971,14 @@
       <c r="H79" s="4">
         <v>2001</v>
       </c>
-      <c r="I79" s="12"/>
-      <c r="J79" s="13" t="s">
+      <c r="J79" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K79" s="12" t="s">
+      <c r="K79" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="80" spans="1:11">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>63</v>
       </c>
@@ -2902,15 +2998,14 @@
       <c r="H80" s="4">
         <v>2001</v>
       </c>
-      <c r="I80" s="12"/>
-      <c r="J80" s="13" t="s">
+      <c r="J80" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K80" s="12" t="s">
+      <c r="K80" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="81" spans="1:20">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>63</v>
       </c>
@@ -2930,15 +3025,14 @@
       <c r="H81" s="4">
         <v>2001</v>
       </c>
-      <c r="I81" s="12"/>
-      <c r="J81" s="13" t="s">
+      <c r="J81" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K81" s="12" t="s">
+      <c r="K81" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="82" spans="1:20">
+    <row r="82" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>63</v>
       </c>
@@ -2958,15 +3052,14 @@
       <c r="H82" s="4">
         <v>2001</v>
       </c>
-      <c r="I82" s="12"/>
-      <c r="J82" s="13" t="s">
+      <c r="J82" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K82" s="12" t="s">
+      <c r="K82" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="83" spans="1:20">
+    <row r="83" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>63</v>
       </c>
@@ -2986,15 +3079,14 @@
       <c r="H83" s="4">
         <v>2001</v>
       </c>
-      <c r="I83" s="12"/>
-      <c r="J83" s="13" t="s">
+      <c r="J83" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K83" s="12" t="s">
+      <c r="K83" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="84" spans="1:20">
+    <row r="84" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>63</v>
       </c>
@@ -3014,15 +3106,14 @@
       <c r="H84" s="4">
         <v>2001</v>
       </c>
-      <c r="I84" s="12"/>
-      <c r="J84" s="13" t="s">
+      <c r="J84" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K84" s="12" t="s">
+      <c r="K84" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="85" spans="1:20">
+    <row r="85" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>63</v>
       </c>
@@ -3042,15 +3133,14 @@
       <c r="H85" s="4">
         <v>2001</v>
       </c>
-      <c r="I85" s="12"/>
-      <c r="J85" s="13" t="s">
+      <c r="J85" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K85" s="12" t="s">
+      <c r="K85" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="86" spans="1:20">
+    <row r="86" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>63</v>
       </c>
@@ -3070,18 +3160,17 @@
       <c r="H86" s="4">
         <v>2001</v>
       </c>
-      <c r="I86" s="12"/>
-      <c r="J86" s="13" t="s">
+      <c r="J86" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K86" s="12" t="s">
+      <c r="K86" t="s">
         <v>91</v>
       </c>
       <c r="R86" s="1"/>
       <c r="S86" s="1"/>
       <c r="T86" s="1"/>
     </row>
-    <row r="87" spans="1:20">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>63</v>
       </c>
@@ -3108,7 +3197,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="88" spans="1:20">
+    <row r="88" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>63</v>
       </c>
@@ -3135,7 +3224,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="89" spans="1:20">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>63</v>
       </c>
@@ -3165,7 +3254,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="90" spans="1:20">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>63</v>
       </c>
@@ -3195,7 +3284,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="91" spans="1:20">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>63</v>
       </c>
@@ -3225,7 +3314,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="92" spans="1:20">
+    <row r="92" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>63</v>
       </c>
@@ -3255,7 +3344,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="93" spans="1:20">
+    <row r="93" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>63</v>
       </c>
@@ -3285,7 +3374,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="94" spans="1:20">
+    <row r="94" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>63</v>
       </c>
@@ -3315,7 +3404,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="95" spans="1:20">
+    <row r="95" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>63</v>
       </c>
@@ -3345,7 +3434,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="96" spans="1:20">
+    <row r="96" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>63</v>
       </c>
@@ -3375,7 +3464,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="97" spans="1:11">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>63</v>
       </c>
@@ -3405,7 +3494,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="98" spans="1:11">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>63</v>
       </c>
@@ -3435,7 +3524,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="99" spans="1:11">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>18</v>
       </c>
@@ -3462,7 +3551,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="100" spans="1:11">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>18</v>
       </c>
@@ -3489,7 +3578,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="101" spans="1:11">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>18</v>
       </c>
@@ -3516,7 +3605,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="102" spans="1:11">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>18</v>
       </c>
@@ -3543,7 +3632,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="103" spans="1:11">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>18</v>
       </c>
@@ -3570,7 +3659,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="104" spans="1:11">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>19</v>
       </c>
@@ -3597,7 +3686,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="105" spans="1:11">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>19</v>
       </c>
@@ -3624,7 +3713,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="106" spans="1:11">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>20</v>
       </c>
@@ -3654,7 +3743,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="107" spans="1:11">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>20</v>
       </c>
@@ -3684,7 +3773,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="108" spans="1:11">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>20</v>
       </c>
@@ -3714,7 +3803,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="109" spans="1:11">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>21</v>
       </c>
@@ -3744,7 +3833,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="110" spans="1:11">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>21</v>
       </c>
@@ -3774,7 +3863,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="111" spans="1:11">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>21</v>
       </c>
@@ -3804,7 +3893,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="112" spans="1:11">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>21</v>
       </c>
@@ -3834,7 +3923,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="113" spans="1:11">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>21</v>
       </c>
@@ -3858,7 +3947,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="114" spans="1:11">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>21</v>
       </c>
@@ -3882,7 +3971,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="115" spans="1:11">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>21</v>
       </c>
@@ -3906,7 +3995,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="116" spans="1:11">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>21</v>
       </c>
@@ -3930,7 +4019,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="117" spans="1:11">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>22</v>
       </c>
@@ -3957,7 +4046,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="118" spans="1:11">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>22</v>
       </c>
@@ -3984,7 +4073,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="119" spans="1:11">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>23</v>
       </c>
@@ -4011,7 +4100,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="120" spans="1:11">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>23</v>
       </c>
@@ -4038,7 +4127,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="121" spans="1:11">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>23</v>
       </c>
@@ -4065,7 +4154,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="122" spans="1:11">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>23</v>
       </c>
@@ -4095,7 +4184,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="123" spans="1:11">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>23</v>
       </c>
@@ -4125,7 +4214,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="124" spans="1:11">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>23</v>
       </c>
@@ -4152,7 +4241,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="125" spans="1:11">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>57</v>
       </c>
@@ -4177,7 +4266,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="126" spans="1:11">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>24</v>
       </c>
@@ -4194,15 +4283,14 @@
       <c r="G126" s="4">
         <v>2017</v>
       </c>
-      <c r="I126" s="12">
+      <c r="I126">
         <v>5</v>
       </c>
-      <c r="J126" s="13" t="s">
+      <c r="J126" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="K126" s="12"/>
-    </row>
-    <row r="127" spans="1:11">
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>25</v>
       </c>
@@ -4219,15 +4307,14 @@
       <c r="G127" s="4">
         <v>2017</v>
       </c>
-      <c r="I127" s="12">
+      <c r="I127">
         <v>5</v>
       </c>
-      <c r="J127" s="13" t="s">
+      <c r="J127" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="K127" s="12"/>
-    </row>
-    <row r="128" spans="1:11">
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>26</v>
       </c>
@@ -4252,7 +4339,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="129" spans="1:11">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>26</v>
       </c>
@@ -4279,7 +4366,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="130" spans="1:11">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>26</v>
       </c>
@@ -4306,7 +4393,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="131" spans="1:11">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>26</v>
       </c>
@@ -4333,7 +4420,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="132" spans="1:11">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>26</v>
       </c>
@@ -4360,77 +4447,77 @@
         <v>60</v>
       </c>
     </row>
-    <row r="133" spans="1:11">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
       <c r="D133" s="1"/>
       <c r="G133" s="1"/>
     </row>
-    <row r="134" spans="1:11">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
       <c r="D134" s="1"/>
       <c r="G134" s="1"/>
     </row>
-    <row r="135" spans="1:11">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
       <c r="D135" s="1"/>
       <c r="G135" s="1"/>
     </row>
-    <row r="136" spans="1:11">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
       <c r="D136" s="1"/>
       <c r="G136" s="1"/>
     </row>
-    <row r="137" spans="1:11">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
       <c r="D137" s="1"/>
       <c r="G137" s="1"/>
     </row>
-    <row r="138" spans="1:11">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
       <c r="D138" s="1"/>
       <c r="G138" s="1"/>
     </row>
-    <row r="139" spans="1:11">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
       <c r="D139" s="1"/>
       <c r="G139" s="1"/>
     </row>
-    <row r="140" spans="1:11">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
       <c r="D140" s="1"/>
       <c r="G140" s="1"/>
     </row>
-    <row r="141" spans="1:11">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
       <c r="D141" s="1"/>
       <c r="G141" s="1"/>
     </row>
-    <row r="142" spans="1:11">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
       <c r="D142" s="1"/>
       <c r="G142" s="1"/>
     </row>
-    <row r="143" spans="1:11">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A143" s="1"/>
       <c r="C143" s="1"/>
       <c r="D143" s="1"/>
@@ -4439,4 +4526,132 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{080C1CE6-9A1E-5842-99F8-EF78431AC316}">
+  <dimension ref="B3:G16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="43.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:7" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="16"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B5" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B6" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B7" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B8" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B9" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B10" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B11" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B12" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B13" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="B14" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="B15" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="B16" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:C3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>